<commit_message>
created hashtable and hashmap
</commit_message>
<xml_diff>
--- a/Recources/meet.xlsx
+++ b/Recources/meet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14595" windowHeight="6960"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14595" windowHeight="8895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>title</t>
   </si>
@@ -50,6 +50,39 @@
   </si>
   <si>
     <t>meetingbook</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>emails</t>
+  </si>
+  <si>
+    <t>Friday afternoon meeting</t>
+  </si>
+  <si>
+    <t>bg5@mailinator.com</t>
+  </si>
+  <si>
+    <t>meetfromicon</t>
+  </si>
+  <si>
+    <t>Afterlunch meeting</t>
+  </si>
+  <si>
+    <t>bg8@mailinator.com</t>
+  </si>
+  <si>
+    <t>Onsite meeting</t>
+  </si>
+  <si>
+    <t>bg10@mailinator.com</t>
+  </si>
+  <si>
+    <t>Offshore meeting</t>
+  </si>
+  <si>
+    <t>bg12@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -392,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,9 +492,56 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>